<commit_message>
Add [API Design] Change password & Search user name
</commit_message>
<xml_diff>
--- a/doc/backend/api/TRN-MiniBlog_API-Specification_TuanNguyen.xlsx
+++ b/doc/backend/api/TRN-MiniBlog_API-Specification_TuanNguyen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="25605" windowHeight="14085" tabRatio="957" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="25605" windowHeight="14085" tabRatio="957" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="23" r:id="rId1"/>
@@ -2167,44 +2167,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="280" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2236,16 +2240,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2273,21 +2267,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2300,45 +2279,66 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2363,10 +2363,19 @@
     <xf numFmtId="49" fontId="13" fillId="8" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2386,26 +2395,17 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="411">
@@ -2846,8 +2846,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>177799</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2856,8 +2856,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1879600" y="1035050"/>
-          <a:ext cx="6461125" cy="2711449"/>
+          <a:off x="1885950" y="1038225"/>
+          <a:ext cx="6486525" cy="2924175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2946,12 +2946,47 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>      "description" : "Succcess",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>      "messages" : {</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>      "message": "Success"</a:t>
-          </a:r>
+            <a:t>      	"message": "Success"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>      }</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -3177,8 +3212,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3188,7 +3223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1847850" y="4381500"/>
-          <a:ext cx="6534150" cy="1590675"/>
+          <a:ext cx="6534150" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3281,13 +3316,42 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>      "message": "Database</a:t>
+            <a:t>      "description"</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
+            <a:t> : "Database error",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>      "messages" : {</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>	"message": "Database</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
             <a:t> error occured. Please try again later.</a:t>
           </a:r>
           <a:r>
@@ -3296,6 +3360,15 @@
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:t>"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>      }</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5163,305 +5236,305 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="43" customFormat="1" ht="15.75">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="199" t="s">
+      <c r="B1" s="166"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="204" t="s">
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="170" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="205"/>
-      <c r="M1" s="206"/>
-      <c r="N1" s="186" t="s">
+      <c r="L1" s="171"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="173" t="s">
         <v>157</v>
       </c>
-      <c r="O1" s="187"/>
-      <c r="P1" s="187"/>
-      <c r="Q1" s="187"/>
-      <c r="R1" s="187"/>
-      <c r="S1" s="187"/>
-      <c r="T1" s="187"/>
-      <c r="U1" s="188"/>
-      <c r="V1" s="207" t="s">
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174"/>
+      <c r="U1" s="175"/>
+      <c r="V1" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="208"/>
-      <c r="X1" s="208"/>
-      <c r="Y1" s="208"/>
-      <c r="Z1" s="208"/>
-      <c r="AA1" s="208"/>
-      <c r="AB1" s="208"/>
-      <c r="AC1" s="208"/>
-      <c r="AD1" s="209"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="178"/>
     </row>
     <row r="2" spans="1:30" s="43" customFormat="1" ht="15.75">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="165" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="199" t="s">
+      <c r="B2" s="166"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="168" t="s">
         <v>159</v>
       </c>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="200"/>
-      <c r="K2" s="181" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="182"/>
-      <c r="M2" s="183"/>
-      <c r="N2" s="201" t="s">
+      <c r="L2" s="183"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="194" t="s">
         <v>161</v>
       </c>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
-      <c r="Q2" s="202"/>
-      <c r="R2" s="202"/>
-      <c r="S2" s="202"/>
-      <c r="T2" s="202"/>
-      <c r="U2" s="203"/>
-      <c r="V2" s="178" t="s">
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195"/>
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="196"/>
+      <c r="V2" s="179" t="s">
         <v>163</v>
       </c>
-      <c r="W2" s="179"/>
-      <c r="X2" s="180"/>
-      <c r="Y2" s="178" t="s">
+      <c r="W2" s="180"/>
+      <c r="X2" s="181"/>
+      <c r="Y2" s="179" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="179"/>
-      <c r="AA2" s="180"/>
-      <c r="AB2" s="178" t="s">
+      <c r="Z2" s="180"/>
+      <c r="AA2" s="181"/>
+      <c r="AB2" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="179"/>
-      <c r="AD2" s="180"/>
+      <c r="AC2" s="180"/>
+      <c r="AD2" s="181"/>
     </row>
     <row r="3" spans="1:30" s="43" customFormat="1" ht="15.75">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="182" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="182"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="184" t="s">
+      <c r="B3" s="183"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="185" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="181" t="s">
+      <c r="E3" s="186"/>
+      <c r="F3" s="186"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="186"/>
+      <c r="K3" s="182" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="182"/>
-      <c r="M3" s="183"/>
-      <c r="N3" s="186" t="s">
+      <c r="L3" s="183"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="173" t="s">
         <v>162</v>
       </c>
-      <c r="O3" s="187"/>
-      <c r="P3" s="187"/>
-      <c r="Q3" s="187"/>
-      <c r="R3" s="187"/>
-      <c r="S3" s="187"/>
-      <c r="T3" s="187"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="189" t="s">
+      <c r="O3" s="174"/>
+      <c r="P3" s="174"/>
+      <c r="Q3" s="174"/>
+      <c r="R3" s="174"/>
+      <c r="S3" s="174"/>
+      <c r="T3" s="174"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="187" t="s">
         <v>252</v>
       </c>
-      <c r="W3" s="190"/>
-      <c r="X3" s="191"/>
-      <c r="Y3" s="192" t="s">
+      <c r="W3" s="188"/>
+      <c r="X3" s="189"/>
+      <c r="Y3" s="190" t="s">
         <v>253</v>
       </c>
-      <c r="Z3" s="193"/>
-      <c r="AA3" s="194"/>
-      <c r="AB3" s="195"/>
-      <c r="AC3" s="193"/>
-      <c r="AD3" s="194"/>
+      <c r="Z3" s="191"/>
+      <c r="AA3" s="192"/>
+      <c r="AB3" s="193"/>
+      <c r="AC3" s="191"/>
+      <c r="AD3" s="192"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:30" ht="16.5" thickBot="1">
-      <c r="B8" s="176" t="s">
+      <c r="B8" s="209" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="176"/>
-      <c r="D8" s="176"/>
-      <c r="E8" s="176"/>
-      <c r="F8" s="176" t="s">
+      <c r="C8" s="209"/>
+      <c r="D8" s="209"/>
+      <c r="E8" s="209"/>
+      <c r="F8" s="209" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="176"/>
-      <c r="H8" s="176" t="s">
+      <c r="G8" s="209"/>
+      <c r="H8" s="209" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="176"/>
-      <c r="J8" s="176"/>
-      <c r="K8" s="176" t="s">
+      <c r="I8" s="209"/>
+      <c r="J8" s="209"/>
+      <c r="K8" s="209" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="176"/>
-      <c r="M8" s="176"/>
-      <c r="N8" s="176"/>
-      <c r="O8" s="176"/>
-      <c r="P8" s="176"/>
-      <c r="Q8" s="176"/>
-      <c r="R8" s="176"/>
-      <c r="S8" s="176"/>
-      <c r="T8" s="176"/>
-      <c r="U8" s="176"/>
-      <c r="V8" s="176"/>
-      <c r="W8" s="176"/>
-      <c r="X8" s="176" t="s">
+      <c r="L8" s="209"/>
+      <c r="M8" s="209"/>
+      <c r="N8" s="209"/>
+      <c r="O8" s="209"/>
+      <c r="P8" s="209"/>
+      <c r="Q8" s="209"/>
+      <c r="R8" s="209"/>
+      <c r="S8" s="209"/>
+      <c r="T8" s="209"/>
+      <c r="U8" s="209"/>
+      <c r="V8" s="209"/>
+      <c r="W8" s="209"/>
+      <c r="X8" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="Y8" s="176"/>
-      <c r="Z8" s="176"/>
-      <c r="AA8" s="176"/>
-      <c r="AB8" s="176"/>
-      <c r="AC8" s="176"/>
+      <c r="Y8" s="209"/>
+      <c r="Z8" s="209"/>
+      <c r="AA8" s="209"/>
+      <c r="AB8" s="209"/>
+      <c r="AC8" s="209"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="B9" s="177" t="s">
+      <c r="B9" s="197" t="s">
         <v>253</v>
       </c>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="167"/>
-      <c r="F9" s="168" t="s">
+      <c r="C9" s="198"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="199"/>
+      <c r="F9" s="200" t="s">
         <v>156</v>
       </c>
-      <c r="G9" s="169"/>
-      <c r="H9" s="165" t="s">
+      <c r="G9" s="201"/>
+      <c r="H9" s="202" t="s">
         <v>254</v>
       </c>
-      <c r="I9" s="166"/>
-      <c r="J9" s="167"/>
-      <c r="K9" s="170" t="s">
+      <c r="I9" s="198"/>
+      <c r="J9" s="199"/>
+      <c r="K9" s="203" t="s">
         <v>255</v>
       </c>
-      <c r="L9" s="171"/>
-      <c r="M9" s="171"/>
-      <c r="N9" s="171"/>
-      <c r="O9" s="171"/>
-      <c r="P9" s="171"/>
-      <c r="Q9" s="171"/>
-      <c r="R9" s="171"/>
-      <c r="S9" s="171"/>
-      <c r="T9" s="171"/>
-      <c r="U9" s="171"/>
-      <c r="V9" s="171"/>
-      <c r="W9" s="172"/>
-      <c r="X9" s="173"/>
-      <c r="Y9" s="174"/>
-      <c r="Z9" s="174"/>
-      <c r="AA9" s="174"/>
-      <c r="AB9" s="174"/>
-      <c r="AC9" s="175"/>
+      <c r="L9" s="204"/>
+      <c r="M9" s="204"/>
+      <c r="N9" s="204"/>
+      <c r="O9" s="204"/>
+      <c r="P9" s="204"/>
+      <c r="Q9" s="204"/>
+      <c r="R9" s="204"/>
+      <c r="S9" s="204"/>
+      <c r="T9" s="204"/>
+      <c r="U9" s="204"/>
+      <c r="V9" s="204"/>
+      <c r="W9" s="205"/>
+      <c r="X9" s="206"/>
+      <c r="Y9" s="207"/>
+      <c r="Z9" s="207"/>
+      <c r="AA9" s="207"/>
+      <c r="AB9" s="207"/>
+      <c r="AC9" s="208"/>
     </row>
     <row r="10" spans="1:30">
-      <c r="B10" s="165"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="167"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="167"/>
-      <c r="K10" s="170"/>
-      <c r="L10" s="171"/>
-      <c r="M10" s="171"/>
-      <c r="N10" s="171"/>
-      <c r="O10" s="171"/>
-      <c r="P10" s="171"/>
-      <c r="Q10" s="171"/>
-      <c r="R10" s="171"/>
-      <c r="S10" s="171"/>
-      <c r="T10" s="171"/>
-      <c r="U10" s="171"/>
-      <c r="V10" s="171"/>
-      <c r="W10" s="172"/>
-      <c r="X10" s="173"/>
-      <c r="Y10" s="174"/>
-      <c r="Z10" s="174"/>
-      <c r="AA10" s="174"/>
-      <c r="AB10" s="174"/>
-      <c r="AC10" s="175"/>
+      <c r="B10" s="202"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="202"/>
+      <c r="I10" s="198"/>
+      <c r="J10" s="199"/>
+      <c r="K10" s="203"/>
+      <c r="L10" s="204"/>
+      <c r="M10" s="204"/>
+      <c r="N10" s="204"/>
+      <c r="O10" s="204"/>
+      <c r="P10" s="204"/>
+      <c r="Q10" s="204"/>
+      <c r="R10" s="204"/>
+      <c r="S10" s="204"/>
+      <c r="T10" s="204"/>
+      <c r="U10" s="204"/>
+      <c r="V10" s="204"/>
+      <c r="W10" s="205"/>
+      <c r="X10" s="206"/>
+      <c r="Y10" s="207"/>
+      <c r="Z10" s="207"/>
+      <c r="AA10" s="207"/>
+      <c r="AB10" s="207"/>
+      <c r="AC10" s="208"/>
     </row>
     <row r="11" spans="1:30">
-      <c r="B11" s="165"/>
-      <c r="C11" s="166"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="165"/>
-      <c r="I11" s="166"/>
-      <c r="J11" s="167"/>
-      <c r="K11" s="170"/>
-      <c r="L11" s="171"/>
-      <c r="M11" s="171"/>
-      <c r="N11" s="171"/>
-      <c r="O11" s="171"/>
-      <c r="P11" s="171"/>
-      <c r="Q11" s="171"/>
-      <c r="R11" s="171"/>
-      <c r="S11" s="171"/>
-      <c r="T11" s="171"/>
-      <c r="U11" s="171"/>
-      <c r="V11" s="171"/>
-      <c r="W11" s="172"/>
-      <c r="X11" s="173"/>
-      <c r="Y11" s="174"/>
-      <c r="Z11" s="174"/>
-      <c r="AA11" s="174"/>
-      <c r="AB11" s="174"/>
-      <c r="AC11" s="175"/>
+      <c r="B11" s="202"/>
+      <c r="C11" s="198"/>
+      <c r="D11" s="198"/>
+      <c r="E11" s="199"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="202"/>
+      <c r="I11" s="198"/>
+      <c r="J11" s="199"/>
+      <c r="K11" s="203"/>
+      <c r="L11" s="204"/>
+      <c r="M11" s="204"/>
+      <c r="N11" s="204"/>
+      <c r="O11" s="204"/>
+      <c r="P11" s="204"/>
+      <c r="Q11" s="204"/>
+      <c r="R11" s="204"/>
+      <c r="S11" s="204"/>
+      <c r="T11" s="204"/>
+      <c r="U11" s="204"/>
+      <c r="V11" s="204"/>
+      <c r="W11" s="205"/>
+      <c r="X11" s="206"/>
+      <c r="Y11" s="207"/>
+      <c r="Z11" s="207"/>
+      <c r="AA11" s="207"/>
+      <c r="AB11" s="207"/>
+      <c r="AC11" s="208"/>
     </row>
     <row r="12" spans="1:30">
-      <c r="B12" s="165"/>
-      <c r="C12" s="166"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="167"/>
-      <c r="F12" s="168"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="165"/>
-      <c r="I12" s="166"/>
-      <c r="J12" s="167"/>
-      <c r="K12" s="170"/>
-      <c r="L12" s="171"/>
-      <c r="M12" s="171"/>
-      <c r="N12" s="171"/>
-      <c r="O12" s="171"/>
-      <c r="P12" s="171"/>
-      <c r="Q12" s="171"/>
-      <c r="R12" s="171"/>
-      <c r="S12" s="171"/>
-      <c r="T12" s="171"/>
-      <c r="U12" s="171"/>
-      <c r="V12" s="171"/>
-      <c r="W12" s="172"/>
-      <c r="X12" s="173"/>
-      <c r="Y12" s="174"/>
-      <c r="Z12" s="174"/>
-      <c r="AA12" s="174"/>
-      <c r="AB12" s="174"/>
-      <c r="AC12" s="175"/>
+      <c r="B12" s="202"/>
+      <c r="C12" s="198"/>
+      <c r="D12" s="198"/>
+      <c r="E12" s="199"/>
+      <c r="F12" s="200"/>
+      <c r="G12" s="201"/>
+      <c r="H12" s="202"/>
+      <c r="I12" s="198"/>
+      <c r="J12" s="199"/>
+      <c r="K12" s="203"/>
+      <c r="L12" s="204"/>
+      <c r="M12" s="204"/>
+      <c r="N12" s="204"/>
+      <c r="O12" s="204"/>
+      <c r="P12" s="204"/>
+      <c r="Q12" s="204"/>
+      <c r="R12" s="204"/>
+      <c r="S12" s="204"/>
+      <c r="T12" s="204"/>
+      <c r="U12" s="204"/>
+      <c r="V12" s="204"/>
+      <c r="W12" s="205"/>
+      <c r="X12" s="206"/>
+      <c r="Y12" s="207"/>
+      <c r="Z12" s="207"/>
+      <c r="AA12" s="207"/>
+      <c r="AB12" s="207"/>
+      <c r="AC12" s="208"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1"/>
     <row r="14" spans="1:30" ht="18" customHeight="1"/>
@@ -5491,11 +5564,31 @@
     <row r="38" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:W12"/>
+    <mergeCell ref="X12:AC12"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:W10"/>
+    <mergeCell ref="X10:AC10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:W11"/>
+    <mergeCell ref="X11:AC11"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:W8"/>
+    <mergeCell ref="X8:AC8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:W9"/>
+    <mergeCell ref="X9:AC9"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="A3:C3"/>
@@ -5510,31 +5603,11 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:X2"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:W9"/>
-    <mergeCell ref="X9:AC9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:W8"/>
-    <mergeCell ref="X8:AC8"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:W11"/>
-    <mergeCell ref="X11:AC11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:W10"/>
-    <mergeCell ref="X10:AC10"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:W12"/>
-    <mergeCell ref="X12:AC12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AD1"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6149,8 +6222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -6584,7 +6657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L66"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -6639,10 +6712,10 @@
       <c r="C4" s="104" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="212" t="s">
+      <c r="D4" s="215" t="s">
         <v>223</v>
       </c>
-      <c r="E4" s="212"/>
+      <c r="E4" s="215"/>
       <c r="F4" s="144" t="s">
         <v>221</v>
       </c>
@@ -6660,10 +6733,10 @@
       <c r="C5" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="211" t="s">
+      <c r="D5" s="216" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="211"/>
+      <c r="E5" s="216"/>
       <c r="F5" s="149" t="s">
         <v>224</v>
       </c>
@@ -6718,10 +6791,10 @@
       <c r="C9" s="144" t="s">
         <v>220</v>
       </c>
-      <c r="D9" s="212" t="s">
+      <c r="D9" s="215" t="s">
         <v>223</v>
       </c>
-      <c r="E9" s="212"/>
+      <c r="E9" s="215"/>
       <c r="F9" s="144" t="s">
         <v>221</v>
       </c>
@@ -6733,8 +6806,8 @@
       <c r="C10" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="210"/>
-      <c r="E10" s="210"/>
+      <c r="D10" s="214"/>
+      <c r="E10" s="214"/>
       <c r="F10" s="143"/>
       <c r="G10" s="125"/>
       <c r="H10" s="125"/>
@@ -6746,8 +6819,8 @@
       <c r="C11" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="210"/>
-      <c r="E11" s="210"/>
+      <c r="D11" s="214"/>
+      <c r="E11" s="214"/>
       <c r="F11" s="143"/>
       <c r="G11" s="125"/>
       <c r="H11" s="125"/>
@@ -6759,8 +6832,8 @@
       <c r="C12" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="210"/>
-      <c r="E12" s="210"/>
+      <c r="D12" s="214"/>
+      <c r="E12" s="214"/>
       <c r="F12" s="143"/>
       <c r="G12" s="125"/>
       <c r="H12" s="125"/>
@@ -6772,8 +6845,8 @@
       <c r="C13" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="210"/>
-      <c r="E13" s="210"/>
+      <c r="D13" s="214"/>
+      <c r="E13" s="214"/>
       <c r="F13" s="143"/>
       <c r="G13" s="125"/>
       <c r="H13" s="125"/>
@@ -6785,8 +6858,8 @@
       <c r="C14" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="210"/>
-      <c r="E14" s="210"/>
+      <c r="D14" s="214"/>
+      <c r="E14" s="214"/>
       <c r="F14" s="143"/>
       <c r="G14" s="125"/>
       <c r="H14" s="125"/>
@@ -6798,8 +6871,8 @@
       <c r="C15" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="210"/>
-      <c r="E15" s="210"/>
+      <c r="D15" s="214"/>
+      <c r="E15" s="214"/>
       <c r="F15" s="143"/>
       <c r="G15" s="125"/>
       <c r="H15" s="125"/>
@@ -6828,10 +6901,10 @@
       <c r="C19" s="163" t="s">
         <v>220</v>
       </c>
-      <c r="D19" s="215" t="s">
+      <c r="D19" s="212" t="s">
         <v>223</v>
       </c>
-      <c r="E19" s="216"/>
+      <c r="E19" s="213"/>
       <c r="F19" s="163" t="s">
         <v>221</v>
       </c>
@@ -6843,10 +6916,10 @@
       <c r="C20" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="213" t="s">
+      <c r="D20" s="210" t="s">
         <v>249</v>
       </c>
-      <c r="E20" s="214"/>
+      <c r="E20" s="211"/>
       <c r="F20" s="146"/>
       <c r="G20" s="125"/>
       <c r="H20" s="125"/>
@@ -6858,10 +6931,10 @@
       <c r="C21" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="213" t="s">
+      <c r="D21" s="210" t="s">
         <v>250</v>
       </c>
-      <c r="E21" s="214"/>
+      <c r="E21" s="211"/>
       <c r="F21" s="146" t="s">
         <v>247</v>
       </c>
@@ -6875,10 +6948,10 @@
       <c r="C22" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="213" t="s">
+      <c r="D22" s="210" t="s">
         <v>251</v>
       </c>
-      <c r="E22" s="214"/>
+      <c r="E22" s="211"/>
       <c r="F22" s="146" t="s">
         <v>248</v>
       </c>
@@ -6892,8 +6965,8 @@
       <c r="C23" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="213"/>
-      <c r="E23" s="214"/>
+      <c r="D23" s="210"/>
+      <c r="E23" s="211"/>
       <c r="F23" s="146"/>
       <c r="G23" s="125"/>
       <c r="H23" s="125"/>
@@ -6905,8 +6978,8 @@
       <c r="C24" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="213"/>
-      <c r="E24" s="214"/>
+      <c r="D24" s="210"/>
+      <c r="E24" s="211"/>
       <c r="F24" s="146"/>
       <c r="G24" s="125"/>
       <c r="H24" s="125"/>
@@ -6918,8 +6991,8 @@
       <c r="C25" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="213"/>
-      <c r="E25" s="214"/>
+      <c r="D25" s="210"/>
+      <c r="E25" s="211"/>
       <c r="F25" s="146"/>
       <c r="G25" s="125"/>
       <c r="H25" s="125"/>
@@ -6938,10 +7011,10 @@
       <c r="C28" s="144" t="s">
         <v>220</v>
       </c>
-      <c r="D28" s="212" t="s">
+      <c r="D28" s="215" t="s">
         <v>223</v>
       </c>
-      <c r="E28" s="212"/>
+      <c r="E28" s="215"/>
       <c r="F28" s="144" t="s">
         <v>221</v>
       </c>
@@ -6953,8 +7026,8 @@
       <c r="C29" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="211"/>
-      <c r="E29" s="211"/>
+      <c r="D29" s="216"/>
+      <c r="E29" s="216"/>
       <c r="F29" s="150"/>
       <c r="G29" s="125"/>
       <c r="H29" s="125"/>
@@ -6966,8 +7039,8 @@
       <c r="C30" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="210"/>
-      <c r="E30" s="210"/>
+      <c r="D30" s="214"/>
+      <c r="E30" s="214"/>
       <c r="F30" s="146"/>
       <c r="G30" s="125"/>
       <c r="H30" s="125"/>
@@ -6979,8 +7052,8 @@
       <c r="C31" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="210"/>
-      <c r="E31" s="210"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214"/>
       <c r="F31" s="146"/>
       <c r="G31" s="125"/>
       <c r="H31" s="125"/>
@@ -6992,8 +7065,8 @@
       <c r="C32" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="210"/>
-      <c r="E32" s="210"/>
+      <c r="D32" s="214"/>
+      <c r="E32" s="214"/>
       <c r="F32" s="146"/>
       <c r="G32" s="125"/>
       <c r="H32" s="125"/>
@@ -7005,8 +7078,8 @@
       <c r="C33" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="210"/>
-      <c r="E33" s="210"/>
+      <c r="D33" s="214"/>
+      <c r="E33" s="214"/>
       <c r="F33" s="146"/>
       <c r="G33" s="125"/>
       <c r="H33" s="125"/>
@@ -7018,8 +7091,8 @@
       <c r="C34" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="210"/>
-      <c r="E34" s="210"/>
+      <c r="D34" s="214"/>
+      <c r="E34" s="214"/>
       <c r="F34" s="146"/>
       <c r="G34" s="125"/>
       <c r="H34" s="125"/>
@@ -7031,8 +7104,8 @@
       <c r="C35" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="210"/>
-      <c r="E35" s="210"/>
+      <c r="D35" s="214"/>
+      <c r="E35" s="214"/>
       <c r="F35" s="146"/>
       <c r="G35" s="125"/>
       <c r="H35" s="125"/>
@@ -7044,8 +7117,8 @@
       <c r="C36" s="127" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="210"/>
-      <c r="E36" s="210"/>
+      <c r="D36" s="214"/>
+      <c r="E36" s="214"/>
       <c r="F36" s="146"/>
       <c r="G36" s="125"/>
       <c r="H36" s="125"/>
@@ -7057,8 +7130,8 @@
       <c r="C37" s="127" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="210"/>
-      <c r="E37" s="210"/>
+      <c r="D37" s="214"/>
+      <c r="E37" s="214"/>
       <c r="F37" s="146"/>
       <c r="G37" s="125"/>
       <c r="H37" s="125"/>
@@ -7076,10 +7149,10 @@
       <c r="C41" s="157" t="s">
         <v>220</v>
       </c>
-      <c r="D41" s="212" t="s">
+      <c r="D41" s="215" t="s">
         <v>223</v>
       </c>
-      <c r="E41" s="212"/>
+      <c r="E41" s="215"/>
       <c r="F41" s="157" t="s">
         <v>221</v>
       </c>
@@ -7089,8 +7162,8 @@
         <v>1</v>
       </c>
       <c r="C42" s="127"/>
-      <c r="D42" s="210"/>
-      <c r="E42" s="210"/>
+      <c r="D42" s="214"/>
+      <c r="E42" s="214"/>
       <c r="F42" s="146"/>
     </row>
     <row r="43" spans="2:8" ht="15" customHeight="1">
@@ -7100,8 +7173,8 @@
       <c r="C43" s="127" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="210"/>
-      <c r="E43" s="210"/>
+      <c r="D43" s="214"/>
+      <c r="E43" s="214"/>
       <c r="F43" s="146"/>
     </row>
     <row r="44" spans="2:8">
@@ -7111,8 +7184,8 @@
       <c r="C44" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="D44" s="210"/>
-      <c r="E44" s="210"/>
+      <c r="D44" s="214"/>
+      <c r="E44" s="214"/>
       <c r="F44" s="146"/>
     </row>
     <row r="45" spans="2:8">
@@ -7122,8 +7195,8 @@
       <c r="C45" s="127" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="210"/>
-      <c r="E45" s="210"/>
+      <c r="D45" s="214"/>
+      <c r="E45" s="214"/>
       <c r="F45" s="146"/>
     </row>
     <row r="46" spans="2:8">
@@ -7133,8 +7206,8 @@
       <c r="C46" s="127" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="210"/>
-      <c r="E46" s="210"/>
+      <c r="D46" s="214"/>
+      <c r="E46" s="214"/>
       <c r="F46" s="146"/>
     </row>
     <row r="49" spans="2:6" ht="15.75">
@@ -7150,10 +7223,10 @@
       <c r="C50" s="144" t="s">
         <v>220</v>
       </c>
-      <c r="D50" s="212" t="s">
+      <c r="D50" s="215" t="s">
         <v>223</v>
       </c>
-      <c r="E50" s="212"/>
+      <c r="E50" s="215"/>
       <c r="F50" s="144" t="s">
         <v>221</v>
       </c>
@@ -7165,8 +7238,8 @@
       <c r="C51" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="210"/>
-      <c r="E51" s="210"/>
+      <c r="D51" s="214"/>
+      <c r="E51" s="214"/>
       <c r="F51" s="146"/>
     </row>
     <row r="52" spans="2:6" ht="20.100000000000001" customHeight="1">
@@ -7176,8 +7249,8 @@
       <c r="C52" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="D52" s="210"/>
-      <c r="E52" s="210"/>
+      <c r="D52" s="214"/>
+      <c r="E52" s="214"/>
       <c r="F52" s="146"/>
     </row>
     <row r="53" spans="2:6" ht="20.100000000000001" customHeight="1">
@@ -7187,8 +7260,8 @@
       <c r="C53" s="127" t="s">
         <v>97</v>
       </c>
-      <c r="D53" s="210"/>
-      <c r="E53" s="210"/>
+      <c r="D53" s="214"/>
+      <c r="E53" s="214"/>
       <c r="F53" s="146"/>
     </row>
     <row r="54" spans="2:6" ht="20.100000000000001" customHeight="1">
@@ -7198,8 +7271,8 @@
       <c r="C54" s="127" t="s">
         <v>98</v>
       </c>
-      <c r="D54" s="210"/>
-      <c r="E54" s="210"/>
+      <c r="D54" s="214"/>
+      <c r="E54" s="214"/>
       <c r="F54" s="146"/>
     </row>
     <row r="55" spans="2:6" ht="20.100000000000001" customHeight="1">
@@ -7209,8 +7282,8 @@
       <c r="C55" s="127" t="s">
         <v>99</v>
       </c>
-      <c r="D55" s="210"/>
-      <c r="E55" s="210"/>
+      <c r="D55" s="214"/>
+      <c r="E55" s="214"/>
       <c r="F55" s="146"/>
     </row>
     <row r="56" spans="2:6" ht="20.100000000000001" customHeight="1">
@@ -7220,8 +7293,8 @@
       <c r="C56" s="127" t="s">
         <v>100</v>
       </c>
-      <c r="D56" s="210"/>
-      <c r="E56" s="210"/>
+      <c r="D56" s="214"/>
+      <c r="E56" s="214"/>
       <c r="F56" s="146"/>
     </row>
     <row r="57" spans="2:6" ht="20.100000000000001" customHeight="1">
@@ -7231,8 +7304,8 @@
       <c r="C57" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="D57" s="210"/>
-      <c r="E57" s="210"/>
+      <c r="D57" s="214"/>
+      <c r="E57" s="214"/>
       <c r="F57" s="146"/>
     </row>
     <row r="60" spans="2:6" ht="15.75">
@@ -7248,10 +7321,10 @@
       <c r="C61" s="144" t="s">
         <v>220</v>
       </c>
-      <c r="D61" s="212" t="s">
+      <c r="D61" s="215" t="s">
         <v>223</v>
       </c>
-      <c r="E61" s="212"/>
+      <c r="E61" s="215"/>
       <c r="F61" s="144" t="s">
         <v>221</v>
       </c>
@@ -7263,8 +7336,8 @@
       <c r="C62" s="127" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="213"/>
-      <c r="E62" s="214"/>
+      <c r="D62" s="210"/>
+      <c r="E62" s="211"/>
       <c r="F62" s="146"/>
     </row>
     <row r="63" spans="2:6" ht="15" customHeight="1">
@@ -7274,8 +7347,8 @@
       <c r="C63" s="127" t="s">
         <v>104</v>
       </c>
-      <c r="D63" s="213"/>
-      <c r="E63" s="214"/>
+      <c r="D63" s="210"/>
+      <c r="E63" s="211"/>
       <c r="F63" s="146"/>
     </row>
     <row r="64" spans="2:6" ht="15" customHeight="1">
@@ -7285,8 +7358,8 @@
       <c r="C64" s="127" t="s">
         <v>105</v>
       </c>
-      <c r="D64" s="213"/>
-      <c r="E64" s="214"/>
+      <c r="D64" s="210"/>
+      <c r="E64" s="211"/>
       <c r="F64" s="146"/>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1">
@@ -7296,8 +7369,8 @@
       <c r="C65" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="D65" s="213"/>
-      <c r="E65" s="214"/>
+      <c r="D65" s="210"/>
+      <c r="E65" s="211"/>
       <c r="F65" s="146"/>
     </row>
     <row r="66" spans="2:6">
@@ -7307,17 +7380,37 @@
       <c r="C66" s="127" t="s">
         <v>107</v>
       </c>
-      <c r="D66" s="213"/>
-      <c r="E66" s="214"/>
+      <c r="D66" s="210"/>
+      <c r="E66" s="211"/>
       <c r="F66" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D56:E56"/>
@@ -7334,31 +7427,11 @@
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7439,10 +7512,10 @@
       <c r="D4" s="104" t="s">
         <v>174</v>
       </c>
-      <c r="E4" s="215" t="s">
+      <c r="E4" s="212" t="s">
         <v>173</v>
       </c>
-      <c r="F4" s="216"/>
+      <c r="F4" s="213"/>
       <c r="G4" s="104" t="s">
         <v>171</v>
       </c>
@@ -7930,15 +8003,15 @@
       <c r="B4" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="225" t="s">
+      <c r="C4" s="228" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="236"/>
-      <c r="E4" s="236"/>
-      <c r="F4" s="236"/>
-      <c r="G4" s="236"/>
-      <c r="H4" s="236"/>
-      <c r="I4" s="226"/>
+      <c r="D4" s="229"/>
+      <c r="E4" s="229"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="229"/>
+      <c r="H4" s="229"/>
+      <c r="I4" s="227"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
@@ -7951,15 +8024,15 @@
       <c r="B5" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="225" t="s">
+      <c r="C5" s="228" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="236"/>
-      <c r="E5" s="236"/>
-      <c r="F5" s="236"/>
-      <c r="G5" s="236"/>
-      <c r="H5" s="236"/>
-      <c r="I5" s="226"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
+      <c r="G5" s="229"/>
+      <c r="H5" s="229"/>
+      <c r="I5" s="227"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -7993,15 +8066,15 @@
       <c r="B7" s="70" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="225" t="s">
+      <c r="C7" s="228" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="236"/>
-      <c r="E7" s="236"/>
-      <c r="F7" s="236"/>
-      <c r="G7" s="236"/>
-      <c r="H7" s="236"/>
-      <c r="I7" s="226"/>
+      <c r="D7" s="229"/>
+      <c r="E7" s="229"/>
+      <c r="F7" s="229"/>
+      <c r="G7" s="229"/>
+      <c r="H7" s="229"/>
+      <c r="I7" s="227"/>
       <c r="J7" s="66"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
@@ -8035,15 +8108,15 @@
       <c r="B9" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="C9" s="225" t="s">
+      <c r="C9" s="228" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="236"/>
-      <c r="E9" s="236"/>
-      <c r="F9" s="236"/>
-      <c r="G9" s="236"/>
-      <c r="H9" s="236"/>
-      <c r="I9" s="226"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
+      <c r="F9" s="229"/>
+      <c r="G9" s="229"/>
+      <c r="H9" s="229"/>
+      <c r="I9" s="227"/>
       <c r="J9" s="66"/>
       <c r="K9" s="66"/>
       <c r="L9" s="66"/>
@@ -8106,19 +8179,19 @@
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="232" t="s">
+      <c r="B13" s="235" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="233"/>
-      <c r="J13" s="233"/>
-      <c r="K13" s="233"/>
-      <c r="L13" s="234"/>
+      <c r="C13" s="236"/>
+      <c r="D13" s="236"/>
+      <c r="E13" s="236"/>
+      <c r="F13" s="236"/>
+      <c r="G13" s="236"/>
+      <c r="H13" s="236"/>
+      <c r="I13" s="236"/>
+      <c r="J13" s="236"/>
+      <c r="K13" s="236"/>
+      <c r="L13" s="237"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
@@ -8147,11 +8220,11 @@
       <c r="I14" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="242" t="s">
+      <c r="J14" s="225" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="242"/>
-      <c r="L14" s="242"/>
+      <c r="K14" s="225"/>
+      <c r="L14" s="225"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
@@ -8180,11 +8253,11 @@
       <c r="I15" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="J15" s="235" t="s">
+      <c r="J15" s="238" t="s">
         <v>180</v>
       </c>
-      <c r="K15" s="235"/>
-      <c r="L15" s="235"/>
+      <c r="K15" s="238"/>
+      <c r="L15" s="238"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
@@ -8213,11 +8286,11 @@
       <c r="I16" s="81" t="s">
         <v>246</v>
       </c>
-      <c r="J16" s="235" t="s">
+      <c r="J16" s="238" t="s">
         <v>183</v>
       </c>
-      <c r="K16" s="235"/>
-      <c r="L16" s="235"/>
+      <c r="K16" s="238"/>
+      <c r="L16" s="238"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
@@ -8279,11 +8352,11 @@
       <c r="I18" s="79" t="s">
         <v>261</v>
       </c>
-      <c r="J18" s="225" t="s">
+      <c r="J18" s="228" t="s">
         <v>190</v>
       </c>
-      <c r="K18" s="236"/>
-      <c r="L18" s="226"/>
+      <c r="K18" s="229"/>
+      <c r="L18" s="227"/>
       <c r="M18" s="66"/>
       <c r="N18" s="66"/>
       <c r="O18" s="66"/>
@@ -8312,11 +8385,11 @@
       <c r="I19" s="164" t="s">
         <v>262</v>
       </c>
-      <c r="J19" s="225" t="s">
+      <c r="J19" s="228" t="s">
         <v>194</v>
       </c>
-      <c r="K19" s="236"/>
-      <c r="L19" s="226"/>
+      <c r="K19" s="229"/>
+      <c r="L19" s="227"/>
       <c r="M19" s="66"/>
       <c r="N19" s="66"/>
       <c r="O19" s="66"/>
@@ -8478,11 +8551,11 @@
     </row>
     <row r="29" spans="1:15" s="89" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="69"/>
-      <c r="B29" s="237" t="s">
+      <c r="B29" s="239" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="237"/>
-      <c r="D29" s="237"/>
+      <c r="C29" s="239"/>
+      <c r="D29" s="239"/>
       <c r="E29" s="87"/>
       <c r="F29" s="88"/>
       <c r="G29" s="87"/>
@@ -8497,12 +8570,12 @@
     </row>
     <row r="30" spans="1:15" s="91" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="90"/>
-      <c r="B30" s="229" t="s">
+      <c r="B30" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="230"/>
-      <c r="D30" s="230"/>
-      <c r="E30" s="231"/>
+      <c r="C30" s="233"/>
+      <c r="D30" s="233"/>
+      <c r="E30" s="234"/>
       <c r="F30" s="76" t="s">
         <v>132</v>
       </c>
@@ -8594,10 +8667,10 @@
       <c r="A33" s="66"/>
       <c r="B33" s="92"/>
       <c r="C33" s="97"/>
-      <c r="D33" s="225" t="s">
+      <c r="D33" s="228" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="226"/>
+      <c r="E33" s="227"/>
       <c r="F33" s="78" t="s">
         <v>148</v>
       </c>
@@ -8658,10 +8731,10 @@
       <c r="A35" s="66"/>
       <c r="B35" s="92"/>
       <c r="C35" s="99"/>
-      <c r="D35" s="225" t="s">
+      <c r="D35" s="228" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="226"/>
+      <c r="E35" s="227"/>
       <c r="F35" s="78" t="s">
         <v>202</v>
       </c>
@@ -8724,10 +8797,10 @@
       <c r="A37" s="66"/>
       <c r="B37" s="92"/>
       <c r="C37" s="102"/>
-      <c r="D37" s="225" t="s">
+      <c r="D37" s="228" t="s">
         <v>204</v>
       </c>
-      <c r="E37" s="226"/>
+      <c r="E37" s="227"/>
       <c r="F37" s="78" t="s">
         <v>206</v>
       </c>
@@ -8757,10 +8830,10 @@
       <c r="A38" s="66"/>
       <c r="B38" s="92"/>
       <c r="C38" s="102"/>
-      <c r="D38" s="227" t="s">
+      <c r="D38" s="230" t="s">
         <v>177</v>
       </c>
-      <c r="E38" s="228"/>
+      <c r="E38" s="231"/>
       <c r="F38" s="78" t="s">
         <v>240</v>
       </c>
@@ -8790,10 +8863,10 @@
       <c r="A39" s="66"/>
       <c r="B39" s="92"/>
       <c r="C39" s="97"/>
-      <c r="D39" s="225" t="s">
+      <c r="D39" s="228" t="s">
         <v>191</v>
       </c>
-      <c r="E39" s="226"/>
+      <c r="E39" s="227"/>
       <c r="F39" s="78" t="s">
         <v>238</v>
       </c>
@@ -8889,10 +8962,10 @@
       <c r="A42" s="66"/>
       <c r="B42" s="98"/>
       <c r="C42" s="99"/>
-      <c r="D42" s="225" t="s">
+      <c r="D42" s="228" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="226"/>
+      <c r="E42" s="227"/>
       <c r="F42" s="78" t="s">
         <v>150</v>
       </c>
@@ -9228,11 +9301,11 @@
     </row>
     <row r="61" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="66"/>
-      <c r="B61" s="238" t="s">
+      <c r="B61" s="240" t="s">
         <v>152</v>
       </c>
-      <c r="C61" s="238"/>
-      <c r="D61" s="238"/>
+      <c r="C61" s="240"/>
+      <c r="D61" s="240"/>
       <c r="E61" s="66"/>
       <c r="F61" s="66"/>
       <c r="G61" s="66"/>
@@ -9249,12 +9322,12 @@
     </row>
     <row r="62" spans="1:15" s="91" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="90"/>
-      <c r="B62" s="229" t="s">
+      <c r="B62" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="C62" s="230"/>
-      <c r="D62" s="230"/>
-      <c r="E62" s="231"/>
+      <c r="C62" s="233"/>
+      <c r="D62" s="233"/>
+      <c r="E62" s="234"/>
       <c r="F62" s="76" t="s">
         <v>132</v>
       </c>
@@ -9346,10 +9419,10 @@
       <c r="A65" s="66"/>
       <c r="B65" s="92"/>
       <c r="C65" s="97"/>
-      <c r="D65" s="239" t="s">
+      <c r="D65" s="226" t="s">
         <v>200</v>
       </c>
-      <c r="E65" s="226"/>
+      <c r="E65" s="227"/>
       <c r="F65" s="78" t="s">
         <v>148</v>
       </c>
@@ -9379,10 +9452,10 @@
       <c r="A66" s="66"/>
       <c r="B66" s="92"/>
       <c r="C66" s="97"/>
-      <c r="D66" s="239" t="s">
+      <c r="D66" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="E66" s="240"/>
+      <c r="E66" s="241"/>
       <c r="F66" s="151" t="s">
         <v>226</v>
       </c>
@@ -9412,10 +9485,10 @@
       <c r="A67" s="66"/>
       <c r="B67" s="92"/>
       <c r="C67" s="97"/>
-      <c r="D67" s="241" t="s">
+      <c r="D67" s="242" t="s">
         <v>231</v>
       </c>
-      <c r="E67" s="240"/>
+      <c r="E67" s="241"/>
       <c r="F67" s="151" t="s">
         <v>229</v>
       </c>
@@ -9509,8 +9582,8 @@
       <c r="A70" s="66"/>
       <c r="B70" s="98"/>
       <c r="C70" s="99"/>
-      <c r="D70" s="225"/>
-      <c r="E70" s="226"/>
+      <c r="D70" s="228"/>
+      <c r="E70" s="227"/>
       <c r="F70" s="78"/>
       <c r="G70" s="80"/>
       <c r="H70" s="80"/>
@@ -9900,17 +9973,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B62:E62"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B30:E30"/>
@@ -9924,6 +9986,17 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="D67:E67"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B62:E62"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <hyperlinks>
@@ -9946,7 +10019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -10029,15 +10102,15 @@
       <c r="B4" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="225" t="s">
+      <c r="C4" s="228" t="s">
         <v>242</v>
       </c>
-      <c r="D4" s="236"/>
-      <c r="E4" s="236"/>
-      <c r="F4" s="236"/>
-      <c r="G4" s="236"/>
-      <c r="H4" s="236"/>
-      <c r="I4" s="226"/>
+      <c r="D4" s="229"/>
+      <c r="E4" s="229"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="229"/>
+      <c r="H4" s="229"/>
+      <c r="I4" s="227"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
@@ -10050,15 +10123,15 @@
       <c r="B5" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="225" t="s">
+      <c r="C5" s="228" t="s">
         <v>243</v>
       </c>
-      <c r="D5" s="236"/>
-      <c r="E5" s="236"/>
-      <c r="F5" s="236"/>
-      <c r="G5" s="236"/>
-      <c r="H5" s="236"/>
-      <c r="I5" s="226"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
+      <c r="G5" s="229"/>
+      <c r="H5" s="229"/>
+      <c r="I5" s="227"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -10092,15 +10165,15 @@
       <c r="B7" s="70" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="225" t="s">
+      <c r="C7" s="228" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="236"/>
-      <c r="E7" s="236"/>
-      <c r="F7" s="236"/>
-      <c r="G7" s="236"/>
-      <c r="H7" s="236"/>
-      <c r="I7" s="226"/>
+      <c r="D7" s="229"/>
+      <c r="E7" s="229"/>
+      <c r="F7" s="229"/>
+      <c r="G7" s="229"/>
+      <c r="H7" s="229"/>
+      <c r="I7" s="227"/>
       <c r="J7" s="66"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
@@ -10134,15 +10207,15 @@
       <c r="B9" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="C9" s="225" t="s">
+      <c r="C9" s="228" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="236"/>
-      <c r="E9" s="236"/>
-      <c r="F9" s="236"/>
-      <c r="G9" s="236"/>
-      <c r="H9" s="236"/>
-      <c r="I9" s="226"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
+      <c r="F9" s="229"/>
+      <c r="G9" s="229"/>
+      <c r="H9" s="229"/>
+      <c r="I9" s="227"/>
       <c r="J9" s="66"/>
       <c r="K9" s="66"/>
       <c r="L9" s="66"/>
@@ -10205,19 +10278,19 @@
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="232" t="s">
+      <c r="B13" s="235" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="233"/>
-      <c r="J13" s="233"/>
-      <c r="K13" s="233"/>
-      <c r="L13" s="234"/>
+      <c r="C13" s="236"/>
+      <c r="D13" s="236"/>
+      <c r="E13" s="236"/>
+      <c r="F13" s="236"/>
+      <c r="G13" s="236"/>
+      <c r="H13" s="236"/>
+      <c r="I13" s="236"/>
+      <c r="J13" s="236"/>
+      <c r="K13" s="236"/>
+      <c r="L13" s="237"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
@@ -10246,11 +10319,11 @@
       <c r="I14" s="162" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="242" t="s">
+      <c r="J14" s="225" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="242"/>
-      <c r="L14" s="242"/>
+      <c r="K14" s="225"/>
+      <c r="L14" s="225"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
@@ -10279,11 +10352,11 @@
       <c r="I15" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="J15" s="235" t="s">
+      <c r="J15" s="238" t="s">
         <v>180</v>
       </c>
-      <c r="K15" s="235"/>
-      <c r="L15" s="235"/>
+      <c r="K15" s="238"/>
+      <c r="L15" s="238"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
@@ -10312,11 +10385,11 @@
       <c r="I16" s="81" t="s">
         <v>246</v>
       </c>
-      <c r="J16" s="235" t="s">
+      <c r="J16" s="238" t="s">
         <v>181</v>
       </c>
-      <c r="K16" s="235"/>
-      <c r="L16" s="235"/>
+      <c r="K16" s="238"/>
+      <c r="L16" s="238"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
@@ -10348,9 +10421,9 @@
       <c r="G18" s="80"/>
       <c r="H18" s="80"/>
       <c r="I18" s="79"/>
-      <c r="J18" s="225"/>
-      <c r="K18" s="236"/>
-      <c r="L18" s="226"/>
+      <c r="J18" s="228"/>
+      <c r="K18" s="229"/>
+      <c r="L18" s="227"/>
       <c r="M18" s="66"/>
       <c r="N18" s="66"/>
       <c r="O18" s="66"/>
@@ -10365,9 +10438,9 @@
       <c r="G19" s="80"/>
       <c r="H19" s="80"/>
       <c r="I19" s="83"/>
-      <c r="J19" s="225"/>
-      <c r="K19" s="236"/>
-      <c r="L19" s="226"/>
+      <c r="J19" s="228"/>
+      <c r="K19" s="229"/>
+      <c r="L19" s="227"/>
       <c r="M19" s="66"/>
       <c r="N19" s="66"/>
       <c r="O19" s="66"/>
@@ -10529,11 +10602,11 @@
     </row>
     <row r="29" spans="1:15" s="89" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="69"/>
-      <c r="B29" s="237" t="s">
+      <c r="B29" s="239" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="237"/>
-      <c r="D29" s="237"/>
+      <c r="C29" s="239"/>
+      <c r="D29" s="239"/>
       <c r="E29" s="87"/>
       <c r="F29" s="88"/>
       <c r="G29" s="87"/>
@@ -10548,12 +10621,12 @@
     </row>
     <row r="30" spans="1:15" s="91" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="90"/>
-      <c r="B30" s="229" t="s">
+      <c r="B30" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="230"/>
-      <c r="D30" s="230"/>
-      <c r="E30" s="231"/>
+      <c r="C30" s="233"/>
+      <c r="D30" s="233"/>
+      <c r="E30" s="234"/>
       <c r="F30" s="162" t="s">
         <v>132</v>
       </c>
@@ -10645,10 +10718,10 @@
       <c r="A33" s="66"/>
       <c r="B33" s="92"/>
       <c r="C33" s="97"/>
-      <c r="D33" s="225" t="s">
+      <c r="D33" s="228" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="226"/>
+      <c r="E33" s="227"/>
       <c r="F33" s="78" t="s">
         <v>148</v>
       </c>
@@ -10709,10 +10782,10 @@
       <c r="A35" s="66"/>
       <c r="B35" s="92"/>
       <c r="C35" s="99"/>
-      <c r="D35" s="225" t="s">
+      <c r="D35" s="228" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="226"/>
+      <c r="E35" s="227"/>
       <c r="F35" s="78" t="s">
         <v>202</v>
       </c>
@@ -10775,10 +10848,10 @@
       <c r="A37" s="66"/>
       <c r="B37" s="98"/>
       <c r="C37" s="99"/>
-      <c r="D37" s="225" t="s">
+      <c r="D37" s="228" t="s">
         <v>149</v>
       </c>
-      <c r="E37" s="226"/>
+      <c r="E37" s="227"/>
       <c r="F37" s="78" t="s">
         <v>150</v>
       </c>
@@ -11114,11 +11187,11 @@
     </row>
     <row r="56" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="66"/>
-      <c r="B56" s="238" t="s">
+      <c r="B56" s="240" t="s">
         <v>152</v>
       </c>
-      <c r="C56" s="238"/>
-      <c r="D56" s="238"/>
+      <c r="C56" s="240"/>
+      <c r="D56" s="240"/>
       <c r="E56" s="66"/>
       <c r="F56" s="66"/>
       <c r="G56" s="66"/>
@@ -11135,12 +11208,12 @@
     </row>
     <row r="57" spans="1:15" s="91" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="90"/>
-      <c r="B57" s="229" t="s">
+      <c r="B57" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="C57" s="230"/>
-      <c r="D57" s="230"/>
-      <c r="E57" s="231"/>
+      <c r="C57" s="233"/>
+      <c r="D57" s="233"/>
+      <c r="E57" s="234"/>
       <c r="F57" s="162" t="s">
         <v>132</v>
       </c>
@@ -11232,10 +11305,10 @@
       <c r="A60" s="66"/>
       <c r="B60" s="92"/>
       <c r="C60" s="97"/>
-      <c r="D60" s="239" t="s">
+      <c r="D60" s="226" t="s">
         <v>200</v>
       </c>
-      <c r="E60" s="226"/>
+      <c r="E60" s="227"/>
       <c r="F60" s="78" t="s">
         <v>148</v>
       </c>
@@ -11265,10 +11338,10 @@
       <c r="A61" s="66"/>
       <c r="B61" s="92"/>
       <c r="C61" s="97"/>
-      <c r="D61" s="239" t="s">
+      <c r="D61" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="E61" s="240"/>
+      <c r="E61" s="241"/>
       <c r="F61" s="151" t="s">
         <v>226</v>
       </c>
@@ -11298,10 +11371,10 @@
       <c r="A62" s="66"/>
       <c r="B62" s="92"/>
       <c r="C62" s="97"/>
-      <c r="D62" s="241" t="s">
+      <c r="D62" s="242" t="s">
         <v>231</v>
       </c>
-      <c r="E62" s="240"/>
+      <c r="E62" s="241"/>
       <c r="F62" s="151" t="s">
         <v>229</v>
       </c>
@@ -11395,8 +11468,8 @@
       <c r="A65" s="66"/>
       <c r="B65" s="98"/>
       <c r="C65" s="99"/>
-      <c r="D65" s="225"/>
-      <c r="E65" s="226"/>
+      <c r="D65" s="228"/>
+      <c r="E65" s="227"/>
       <c r="F65" s="78"/>
       <c r="G65" s="80"/>
       <c r="H65" s="80"/>
@@ -11786,12 +11859,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="B13:L13"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D35:E35"/>
@@ -11807,6 +11874,12 @@
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="D61:E61"/>
     <mergeCell ref="D62:E62"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I15" r:id="rId1" display="foo@mulodo.com"/>

</xml_diff>